<commit_message>
testing file updated and created details
</commit_message>
<xml_diff>
--- a/version1/manipulating_test_cases.xlsx
+++ b/version1/manipulating_test_cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPR101\CPR101\version1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB19A9D0-C72A-4CAA-9E7F-E1F6301C9FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EF9AD7-B41C-438C-BFC2-AF54EA33CCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t>Program
 or module:</t>
@@ -403,6 +403,26 @@
   </si>
   <si>
     <t>Check if the 2nd string is q as well and exit the program when applicable</t>
+  </si>
+  <si>
+    <t>*** Start of Concatenating Strings Demo ***
+Type the 1st string (q - to quit):
+QbaKozj6CjkH1ATLPQ6rglly9riWzt3nRbrCrrmN5DfMxC8PhwgZSn5vDKdkMPDvBzM2fOJ2lBZum8YbINYUGGlALWwJGGlhK5VQoJ2Xadht4K7hxwb8ChkIbSHdITCdsdHLXm3LL9lwCsWICIb19TNwjrCPwervA43DOAD7KMlnu5lPnWJ4ca9ua4vTUgQ8EwQAKHcg
+Type the 2nd string:
+Concatenated string is 'QbaKozj6CjkH1ATLPQ6rglly9riWzt3nRbrCrrmN5DfMxC8PhwgZSn5vDKdkMPDvBzM2fOJ2lBZum8YbINYUGGlALWwJGGlhK5QoJ2Xadht4K7hxwb8ChkIbSHdITCdsdHLXm3LL9lwCsWICIb19TNwjrCPwervA43DOAD7KMlnu5lPnWJ4ca9ua4vTUgQ8EwQAK'
+Type the 1st string (q - to quit):
+Type the 2nd string:</t>
+  </si>
+  <si>
+    <t>*** Start of Concatenating Strings Demo ***
+Type the 1st string (q - to quit):
+ZyBk27e3yEyMQ0WvL8t6KIJauYhrPmWuyRC2bnNKDcr1ZaScWM7VXZKeSl2u20yTgo0CkBtmuRcJSFdxqTW6r5Kr0hFY5imsxLl0
+Type the 2nd string:
+Concatenated string is 'ZyBk27e3yEyMQ0WvL8t6KIJauYhrPmWuyRC2bnNKDcr1ZaScWM7VXZKeSl2u20yTgo0CkBtmuRcJSFdxqTW6r5Kr0hFY5imsxL0'
+Type the 1st string (q - to quit):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd string input is not being taken , validation should be added here for string 1. </t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1202,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1287,10 +1307,10 @@
         <v>55</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>17</v>
@@ -1537,13 +1557,13 @@
         <v>51</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G15" s="26" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="2"/>
@@ -1841,18 +1861,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2021,18 +2041,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4D9C73-E0F5-404E-9C51-FCAE195853E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC77C8E2-4EFE-4791-A84F-DFECD6468623}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC77C8E2-4EFE-4791-A84F-DFECD6468623}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE4D9C73-E0F5-404E-9C51-FCAE195853E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>